<commit_message>
Popravki sklepcnosti, linki v mailu #3, izboljsave admina
</commit_message>
<xml_diff>
--- a/delegati-tpl.xlsx
+++ b/delegati-tpl.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bostj\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bostj\Desktop\www\sklepnik\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22FC6E45-42E3-4F83-9271-14F13E53C37E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{403E2DD8-E841-4702-970A-0F967CB290E0}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{D0130999-4A4B-4792-B4AB-EEF45AF81BD4}"/>
   </bookViews>
@@ -486,7 +486,7 @@
   <dimension ref="A1:H4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+      <selection activeCell="G26" sqref="G26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>